<commit_message>
new update in oop and assignment 3
</commit_message>
<xml_diff>
--- a/Email Details.xlsx
+++ b/Email Details.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475DEC6A-39C4-48B0-AD76-78ABE5DF746A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB9A7AA-4CD1-4B9E-B509-5664867786C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>Subash Mahat</t>
   </si>
   <si>
-    <t>Subashmahat@gmail.com</t>
-  </si>
-  <si>
     <t>Shradha Maharjan</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>pakhrinreshma@gmail.com</t>
+  </si>
+  <si>
+    <t>Subashmahat35@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A2:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,128 +461,128 @@
         <v>9849899287</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>9801214216</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>9818721210</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>9860479947</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>9849982613</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>9823411889</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>9843935344</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>9813982829</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>9845707933</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>9860297596</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>9823251296</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>9860922735</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>